<commit_message>
Minor change to Excel Table Plan
</commit_message>
<xml_diff>
--- a/table-plan DA.xlsx
+++ b/table-plan DA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2e4684f401fe71c/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\School\Year 4\DTA\Bank Marketing “Term Deposit” Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{56F82D69-8ADC-467F-AEB6-96B1DD481292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55339B68-6122-4B78-9F72-7FAA0871EA5F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CD5C8A-35D5-4E93-BF14-0C833DDA5353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8498482E-B37B-464B-A108-21C576046292}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8498482E-B37B-464B-A108-21C576046292}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -44,9 +33,6 @@
     <t>Task dhe substaks</t>
   </si>
   <si>
-    <t>1.Data understanding and preparation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Load and inspect data </t>
   </si>
   <si>
@@ -137,9 +123,6 @@
     <t>Management Report</t>
   </si>
   <si>
-    <t>revision</t>
-  </si>
-  <si>
     <t>2.5h</t>
   </si>
   <si>
@@ -147,13 +130,19 @@
   </si>
   <si>
     <t>2h</t>
+  </si>
+  <si>
+    <t>1-Data understanding and preparation</t>
+  </si>
+  <si>
+    <t>Revision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,12 +231,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -295,18 +281,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47E7EAD4-C2D5-411D-8410-790B9BE16AD2}" name="Table1" displayName="Table1" ref="E3:M11" totalsRowShown="0">
-  <autoFilter ref="E3:M11" xr:uid="{47E7EAD4-C2D5-411D-8410-790B9BE16AD2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47E7EAD4-C2D5-411D-8410-790B9BE16AD2}" name="Table1" displayName="Table1" ref="A3:I11" totalsRowShown="0">
+  <autoFilter ref="A3:I11" xr:uid="{47E7EAD4-C2D5-411D-8410-790B9BE16AD2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B1AE5FA1-CACA-4538-8627-4075701231E2}" name="Task dhe substaks"/>
-    <tableColumn id="2" xr3:uid="{4198C140-1C6F-4359-8077-F9F8EE4E11CF}" name="1.Data understanding and preparation"/>
+    <tableColumn id="2" xr3:uid="{4198C140-1C6F-4359-8077-F9F8EE4E11CF}" name="1-Data understanding and preparation"/>
     <tableColumn id="3" xr3:uid="{95E09C14-3F6C-4C9A-A3FC-AD90AED74842}" name="EDA"/>
     <tableColumn id="4" xr3:uid="{5FA54A8D-3E56-4227-9DA5-624919C07133}" name="Dataset Setup"/>
     <tableColumn id="5" xr3:uid="{17B1789A-A4D2-4327-BAF3-340E2DAB1834}" name="Baseline Model"/>
     <tableColumn id="6" xr3:uid="{1B650294-64AD-481E-8945-952713C4B5D1}" name="Modeling"/>
     <tableColumn id="7" xr3:uid="{0D47B0AF-C49C-42B1-AE0F-E66B14699036}" name="Model Evaluation"/>
     <tableColumn id="8" xr3:uid="{61C9285C-1D9E-4204-9AA9-49D5798220BC}" name="Final Deliverables"/>
-    <tableColumn id="9" xr3:uid="{FF8D9262-DBEA-48B1-9B99-94C0BF541AA9}" name="revision"/>
+    <tableColumn id="9" xr3:uid="{FF8D9262-DBEA-48B1-9B99-94C0BF541AA9}" name="Revision"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -629,202 +615,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA04B1FC-5049-4B49-A909-0B98CCB3E9D1}">
-  <dimension ref="D2:M12"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="2" customWidth="1"/>
-    <col min="3" max="3" width="8.984375E-2" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" customWidth="1"/>
-    <col min="6" max="6" width="23.08984375" customWidth="1"/>
-    <col min="7" max="7" width="22.08984375" customWidth="1"/>
-    <col min="8" max="8" width="19.36328125" customWidth="1"/>
-    <col min="9" max="9" width="16.90625" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" customWidth="1"/>
-    <col min="11" max="11" width="18.08984375" customWidth="1"/>
-    <col min="12" max="12" width="20.6328125" customWidth="1"/>
-    <col min="13" max="13" width="7.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" customWidth="1"/>
+    <col min="9" max="9" width="16.8984375" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="18.09765625" customWidth="1"/>
+    <col min="12" max="12" width="20.59765625" customWidth="1"/>
+    <col min="13" max="13" width="7.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="5:13" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E3" t="s">
+    <row r="3" spans="1:9" ht="35.549999999999997" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="36" customHeight="1">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="34.5" customHeight="1">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.95" customHeight="1">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="35.549999999999997" customHeight="1">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="39.450000000000003" customHeight="1">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="5:13" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="5:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="5:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E6">
+      <c r="E10" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="39.450000000000003" customHeight="1">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="5:13" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="5:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="5:13" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="5:13" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="6">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="5:13" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="5:13" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="12" spans="1:9" ht="13.95" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>